<commit_message>
Opdateret tidsplan og lavet JSON opsætning dokument
</commit_message>
<xml_diff>
--- a/planlægning/hificorner gantt.xlsx
+++ b/planlægning/hificorner gantt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Kodning_server\Web\Sider\wuhf-hificorner-danieltherkildsen\planlægning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{05C9B744-2BD3-4777-BBA0-3E692090D51F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{300E501D-5603-4CE4-A6EB-E99106FAC847}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -222,34 +222,34 @@
     <t>Activity 31</t>
   </si>
   <si>
-    <t>Header</t>
-  </si>
-  <si>
-    <t>Navigation</t>
-  </si>
-  <si>
     <t>1 point = 1 time</t>
   </si>
   <si>
-    <t>Frontpage Header/nav background w/ logo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Frontpage showroom banner </t>
-  </si>
-  <si>
-    <t>Frontpage product hero slider</t>
-  </si>
-  <si>
-    <t>Frontpage product hero slider funktionalitet</t>
-  </si>
-  <si>
-    <t>Frontpage social box</t>
-  </si>
-  <si>
-    <t>Frontpage social boxes grid</t>
-  </si>
-  <si>
-    <t>Frontpage history/news/shop single item</t>
+    <t>Frontpage product hero slider funktionalitet (JS)</t>
+  </si>
+  <si>
+    <t>Frontpage product hero slider (HTML/CSS)</t>
+  </si>
+  <si>
+    <t>Frontpage Header/nav background w/ logo (HTML/CSS)</t>
+  </si>
+  <si>
+    <t>Frontpage showroom banner (HTML/CSS)</t>
+  </si>
+  <si>
+    <t>Header (HTML/CSS)</t>
+  </si>
+  <si>
+    <t>Navigationw (HTML/CSS)</t>
+  </si>
+  <si>
+    <t>Frontpage social box (HTML/CSS)</t>
+  </si>
+  <si>
+    <t>Frontpage social boxes grid (HTML/CSS)</t>
+  </si>
+  <si>
+    <t>Frontpage history/news/shop single item (HTML/CSS)</t>
   </si>
 </sst>
 </file>
@@ -625,6 +625,15 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="11">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -660,15 +669,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -692,7 +692,7 @@
     <cellStyle name="Project Headers" xfId="4" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
     <cellStyle name="Title" xfId="8" builtinId="15" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="9">
     <dxf>
       <fill>
         <patternFill>
@@ -709,15 +709,6 @@
         <bottom style="thin">
           <color theme="7"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color theme="7"/>
-        </top>
         <vertical/>
         <horizontal/>
       </border>
@@ -1081,14 +1072,14 @@
   </sheetPr>
   <dimension ref="B1:BO35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="R13" sqref="R13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="2.6640625" customWidth="1"/>
-    <col min="2" max="2" width="37.5546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="48.44140625" style="2" customWidth="1"/>
     <col min="3" max="6" width="11.6640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="15.6640625" style="4" customWidth="1"/>
     <col min="8" max="27" width="2.77734375" style="1"/>
@@ -1103,18 +1094,18 @@
       <c r="E1" s="13"/>
       <c r="F1" s="13"/>
       <c r="G1" s="13"/>
-      <c r="H1" s="34" t="s">
-        <v>39</v>
+      <c r="H1" s="22" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
       <c r="G2" s="5" t="s">
         <v>22</v>
       </c>
@@ -1122,66 +1113,66 @@
         <v>1</v>
       </c>
       <c r="J2" s="16"/>
-      <c r="K2" s="30" t="s">
+      <c r="K2" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="32"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
+      <c r="N2" s="34"/>
+      <c r="O2" s="35"/>
       <c r="P2" s="17"/>
-      <c r="Q2" s="30" t="s">
+      <c r="Q2" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="R2" s="31"/>
-      <c r="S2" s="31"/>
-      <c r="T2" s="32"/>
+      <c r="R2" s="34"/>
+      <c r="S2" s="34"/>
+      <c r="T2" s="35"/>
       <c r="U2" s="18"/>
-      <c r="V2" s="22" t="s">
+      <c r="V2" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="W2" s="23"/>
-      <c r="X2" s="23"/>
-      <c r="Y2" s="33"/>
+      <c r="W2" s="26"/>
+      <c r="X2" s="26"/>
+      <c r="Y2" s="36"/>
       <c r="Z2" s="19"/>
-      <c r="AA2" s="22" t="s">
+      <c r="AA2" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="AB2" s="23"/>
-      <c r="AC2" s="23"/>
-      <c r="AD2" s="23"/>
-      <c r="AE2" s="23"/>
-      <c r="AF2" s="23"/>
-      <c r="AG2" s="33"/>
+      <c r="AB2" s="26"/>
+      <c r="AC2" s="26"/>
+      <c r="AD2" s="26"/>
+      <c r="AE2" s="26"/>
+      <c r="AF2" s="26"/>
+      <c r="AG2" s="36"/>
       <c r="AH2" s="20"/>
-      <c r="AI2" s="22" t="s">
+      <c r="AI2" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="AJ2" s="23"/>
-      <c r="AK2" s="23"/>
-      <c r="AL2" s="23"/>
-      <c r="AM2" s="23"/>
-      <c r="AN2" s="23"/>
-      <c r="AO2" s="23"/>
-      <c r="AP2" s="23"/>
+      <c r="AJ2" s="26"/>
+      <c r="AK2" s="26"/>
+      <c r="AL2" s="26"/>
+      <c r="AM2" s="26"/>
+      <c r="AN2" s="26"/>
+      <c r="AO2" s="26"/>
+      <c r="AP2" s="26"/>
     </row>
     <row r="3" spans="2:67" s="12" customFormat="1" ht="39.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="F3" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="G3" s="29" t="s">
+      <c r="G3" s="32" t="s">
         <v>27</v>
       </c>
       <c r="H3" s="21" t="s">
@@ -1208,12 +1199,12 @@
       <c r="AA3" s="11"/>
     </row>
     <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="26"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
       <c r="H4" s="3">
         <v>1</v>
       </c>
@@ -1397,7 +1388,7 @@
     </row>
     <row r="5" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="6" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C5" s="7">
         <v>1</v>
@@ -1417,7 +1408,7 @@
     </row>
     <row r="6" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="6" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C6" s="7">
         <v>2</v>
@@ -1436,7 +1427,7 @@
       </c>
     </row>
     <row r="7" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="23" t="s">
         <v>40</v>
       </c>
       <c r="C7" s="7">
@@ -1456,7 +1447,7 @@
       </c>
     </row>
     <row r="8" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="35" t="s">
+      <c r="B8" s="23" t="s">
         <v>41</v>
       </c>
       <c r="C8" s="7">
@@ -1476,8 +1467,8 @@
       </c>
     </row>
     <row r="9" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="36" t="s">
-        <v>42</v>
+      <c r="B9" s="24" t="s">
+        <v>39</v>
       </c>
       <c r="C9" s="7">
         <v>5</v>
@@ -1496,8 +1487,8 @@
       </c>
     </row>
     <row r="10" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="36" t="s">
-        <v>43</v>
+      <c r="B10" s="24" t="s">
+        <v>38</v>
       </c>
       <c r="C10" s="7">
         <v>6</v>
@@ -2031,28 +2022,28 @@
     <mergeCell ref="AA2:AG2"/>
   </mergeCells>
   <conditionalFormatting sqref="H5:BO35">
-    <cfRule type="expression" dxfId="9" priority="1">
+    <cfRule type="expression" dxfId="8" priority="1">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="3">
+    <cfRule type="expression" dxfId="7" priority="3">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="4">
+    <cfRule type="expression" dxfId="6" priority="4">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="5">
+    <cfRule type="expression" dxfId="5" priority="5">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="6">
+    <cfRule type="expression" dxfId="4" priority="6">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="7">
+    <cfRule type="expression" dxfId="3" priority="7">
       <formula>H$4=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="11">
+    <cfRule type="expression" dxfId="2" priority="11">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="12">
+    <cfRule type="expression" dxfId="1" priority="12">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>